<commit_message>
Update to version 0.10.5.46
</commit_message>
<xml_diff>
--- a/Tasks/Resources/blank_Plan.xlsx
+++ b/Tasks/Resources/blank_Plan.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="План" sheetId="1" r:id="rId1"/>
+    <sheet name="Шаблон" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Описание</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Взаимодействие</t>
+  </si>
+  <si>
+    <t>Основные задачи</t>
   </si>
 </sst>
 </file>
@@ -64,12 +67,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -99,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -116,14 +125,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,56 +438,73 @@
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A5:D5"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>